<commit_message>
feat: 2204 and 2209 = sales forecast
</commit_message>
<xml_diff>
--- a/backend/api/app_templates/sales_forecast_template.xlsx
+++ b/backend/api/app_templates/sales_forecast_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timchen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FEBFDE-D576-784A-8C0D-F0204CF7B892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E120B4CA-5A8F-EA4B-B2C4-07BF75D18D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="2460" windowWidth="27640" windowHeight="16940" xr2:uid="{3E367DA1-2811-4C43-8C2A-70EAFD4D2A2F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Please fill out the "Sales Forecast" sheet</t>
   </si>
@@ -48,55 +48,58 @@
     <t>Please note that:</t>
   </si>
   <si>
-    <t>(1) "model_year" should be an integer</t>
-  </si>
-  <si>
     <t>(2) "make" should be no more than 250 characters</t>
   </si>
   <si>
-    <t>(3) "model_name" should be no more than 250 characters</t>
-  </si>
-  <si>
     <t>(4) "type" should be exactly one of: BEV, PHEV, FCEV, EREV</t>
   </si>
   <si>
     <t>(5) "range" should be a real number with no more than 2 decimal places</t>
   </si>
   <si>
-    <t>(6) "zev_class" should be a single, uppercase letter</t>
-  </si>
-  <si>
-    <t>(7) "interior_volume" should be a real number with no more than 2 decimal places</t>
-  </si>
-  <si>
-    <t>(8) "total_sales" should be an integer</t>
-  </si>
-  <si>
-    <t>model_year</t>
-  </si>
-  <si>
     <t>make</t>
   </si>
   <si>
-    <t>model_name</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
     <t>range</t>
   </si>
   <si>
-    <t>zev_class</t>
-  </si>
-  <si>
-    <t>interior_volume</t>
-  </si>
-  <si>
-    <t>total_sales</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please note that all of the fields in the "Sales Forecast" sheet are mandatory </t>
+  </si>
+  <si>
+    <t>modelYear</t>
+  </si>
+  <si>
+    <t>modelName</t>
+  </si>
+  <si>
+    <t>zevClass</t>
+  </si>
+  <si>
+    <t>interiorVolume</t>
+  </si>
+  <si>
+    <t>totalSales</t>
+  </si>
+  <si>
+    <t>(3) "modelName" should be no more than 250 characters</t>
+  </si>
+  <si>
+    <t>(6) "zevClass" should be a single, uppercase letter</t>
+  </si>
+  <si>
+    <t>(7) "interiorVolume" should be a real number with no more than 2 decimal places</t>
+  </si>
+  <si>
+    <t>(8) "totalSales" should be an integer</t>
+  </si>
+  <si>
+    <t>(1) "modelYear" should be a 4 digit integer</t>
+  </si>
+  <si>
+    <t>Please do not alter the name of the "Sales Forecast" sheet</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3882FB2-E1FB-7145-985F-5D4D3D2256D4}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -484,57 +487,62 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -560,28 +568,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>